<commit_message>
Final version with corrections from draft
</commit_message>
<xml_diff>
--- a/Code and Data/Quick Results.xlsx
+++ b/Code and Data/Quick Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/600dbc9569d8e3d0/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC491348-D622-4E2C-A10A-4377EDBC2D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{AC491348-D622-4E2C-A10A-4377EDBC2D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FE4B362-5D35-45D7-BDC8-AF0D482D9266}"/>
   <bookViews>
-    <workbookView xWindow="34290" yWindow="0" windowWidth="17415" windowHeight="20985" xr2:uid="{97A54175-03F7-418C-9B98-648C062F96A2}"/>
+    <workbookView xWindow="-86" yWindow="0" windowWidth="12617" windowHeight="15823" xr2:uid="{97A54175-03F7-418C-9B98-648C062F96A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>ResNet50</t>
   </si>
@@ -53,24 +53,9 @@
     <t>Improved Student Model</t>
   </si>
   <si>
-    <t>Parameters</t>
-  </si>
-  <si>
     <t>Epochs</t>
   </si>
   <si>
-    <t>Final Accuracy</t>
-  </si>
-  <si>
-    <t>48.8 Million</t>
-  </si>
-  <si>
-    <t>Test Accuracy</t>
-  </si>
-  <si>
-    <t>Test Error</t>
-  </si>
-  <si>
     <t>Fine Tuned</t>
   </si>
   <si>
@@ -80,28 +65,37 @@
     <t>Confusion Matrix reflective</t>
   </si>
   <si>
-    <t>26.1 Million</t>
-  </si>
-  <si>
-    <t>33.6 Million</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
-    <t>19.0 Million</t>
-  </si>
-  <si>
-    <t>5.39 Million</t>
-  </si>
-  <si>
     <t>Model</t>
+  </si>
+  <si>
+    <t>Parameters (Million)</t>
+  </si>
+  <si>
+    <t>Training Accuracy (%)</t>
+  </si>
+  <si>
+    <t>Test Accuracy (%)</t>
+  </si>
+  <si>
+    <t>Test Error (%)</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Average Epoch Time (seconds)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,7 +121,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -309,107 +303,53 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -426,6 +366,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -745,88 +689,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F9718D-BD35-4CDC-877C-331CF56A6476}">
-  <dimension ref="B2:I8"/>
+  <dimension ref="B2:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.53515625" customWidth="1"/>
+    <col min="2" max="2" width="22.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3828125" customWidth="1"/>
+    <col min="4" max="4" width="8.3046875" customWidth="1"/>
+    <col min="5" max="5" width="13.53515625" customWidth="1"/>
+    <col min="6" max="6" width="12.3828125" customWidth="1"/>
+    <col min="7" max="7" width="10.84375" customWidth="1"/>
+    <col min="8" max="8" width="21.69140625" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="16" t="s">
+    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="2:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="J3" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>48.8</v>
+      </c>
+      <c r="D4" s="5">
+        <v>10</v>
+      </c>
+      <c r="E4" s="5">
+        <v>76.95</v>
+      </c>
+      <c r="F4" s="5">
+        <v>67.13</v>
+      </c>
+      <c r="G4" s="5">
+        <v>32.869999999999997</v>
+      </c>
+      <c r="H4" s="5">
+        <f>AVERAGE(154, 86, 83, 87, 80, 81, 85, 62, 79, 78)</f>
+        <v>87.5</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>13</v>
+      <c r="J4" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="8">
-        <v>10</v>
-      </c>
-      <c r="E4" s="8">
-        <v>76.95</v>
-      </c>
-      <c r="F4" s="8">
-        <v>67.13</v>
-      </c>
-      <c r="G4" s="8">
-        <v>32.869999999999997</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>14</v>
+      <c r="C5" s="1">
+        <v>26.1</v>
       </c>
       <c r="D5" s="1">
         <v>10</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>86.67</v>
       </c>
       <c r="F5" s="1">
@@ -835,19 +788,23 @@
       <c r="G5" s="1">
         <v>17.27</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>12</v>
+      <c r="H5" s="1">
+        <f>AVERAGE(129, 61, 79, 39, 35, 35, 44, 37, 35, 38)</f>
+        <v>53.2</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>15</v>
+      <c r="C6" s="1">
+        <v>33.6</v>
       </c>
       <c r="D6" s="1">
         <v>10</v>
@@ -855,25 +812,29 @@
       <c r="E6" s="1">
         <v>9.73</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="14">
         <v>10</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="14">
         <v>90</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>16</v>
+      <c r="H6" s="1">
+        <f>AVERAGE(74, 71, 83, 60, 62, 62, 79, 82, 82, 58)</f>
+        <v>71.3</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>17</v>
+      <c r="C7" s="13">
+        <v>19</v>
       </c>
       <c r="D7" s="1">
         <v>10</v>
@@ -881,43 +842,109 @@
       <c r="E7" s="1">
         <v>91.83</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>76.84</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>23.16</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>12</v>
+      <c r="H7" s="1">
+        <f>AVERAGE(29, 33, 16, 17, 16, 21, 21, 20, 16, 16)</f>
+        <v>20.5</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="C8" s="1">
+        <v>5.39</v>
+      </c>
+      <c r="D8" s="1">
         <v>10</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="1">
         <v>92.77</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="1">
         <v>79.59</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="1">
         <v>20.41</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>12</v>
+      <c r="H8" s="1">
+        <f>AVERAGE(42, 30, 26, 42, 40, 27, 40, 41, 41, 41)</f>
+        <v>37</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5.39</v>
+      </c>
+      <c r="D9" s="1">
+        <v>50</v>
+      </c>
+      <c r="E9" s="1">
+        <v>98.29</v>
+      </c>
+      <c r="F9" s="1">
+        <v>82.98</v>
+      </c>
+      <c r="G9" s="1">
+        <v>17.02</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3">
+        <v>5.39</v>
+      </c>
+      <c r="D10" s="3">
+        <v>100</v>
+      </c>
+      <c r="E10" s="3">
+        <v>98.82</v>
+      </c>
+      <c r="F10" s="3">
+        <v>81.95</v>
+      </c>
+      <c r="G10" s="3">
+        <v>18.05</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>